<commit_message>
Updated test data sheet and added sheet
</commit_message>
<xml_diff>
--- a/Test Data/TC_71687_Verify_Default_Battery_Standby_Load_FC.xlsx
+++ b/Test Data/TC_71687_Verify_Default_Battery_Standby_Load_FC.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029B574A-C80E-43BD-A7AC-1B953CBD1FE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="8" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="31">
   <si>
     <t>Color Codes</t>
   </si>
@@ -112,12 +114,18 @@
   </si>
   <si>
     <t>Standby Current(A)</t>
+  </si>
+  <si>
+    <t>FC702D</t>
+  </si>
+  <si>
+    <t>PFI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,11 +529,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,7 +698,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -699,16 +707,16 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5">
         <v>16</v>
       </c>
       <c r="F10" s="11">
-        <v>0.251</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="G10" s="13">
-        <v>0.439</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="H10" s="5" t="b">
         <v>0</v>
@@ -731,14 +739,227 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE35731F-FD7A-4678-811A-0EC5FA09E652}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5">
+        <v>19</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.39</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5">
+        <v>16</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5">
+        <v>16</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.251</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.439</v>
+      </c>
+      <c r="H10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>

</xml_diff>